<commit_message>
TestDataSheet.xlsx is just opened did not modify
</commit_message>
<xml_diff>
--- a/TestData/TestDataSheet.xlsx
+++ b/TestData/TestDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubCloneRepository\SwarupAnkur1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2230A88-C7E4-42AF-9599-DD0531524C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FE0E8-709B-41E3-B831-8282B9AEE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AAE73E8-762A-4208-8112-C301457E7FD0}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding test data sheet xls and xlsx
</commit_message>
<xml_diff>
--- a/TestData/TestDataSheet.xlsx
+++ b/TestData/TestDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubCloneRepository\SwarupAnkur1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FE0E8-709B-41E3-B831-8282B9AEE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23762DE-F888-40C7-87EC-43B496A53EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AAE73E8-762A-4208-8112-C301457E7FD0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>TCNo</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Swarup3</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Part4</t>
   </si>
 </sst>
 </file>
@@ -94,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,15 +123,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F301094F-715B-4F4F-A876-93CEB5A1FD8B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,6 +521,20 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding two excel file and HelloAnkurSwarup1
</commit_message>
<xml_diff>
--- a/TestData/TestDataSheet.xlsx
+++ b/TestData/TestDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubSwarupAnkur\SwarupTest07\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2166AA-6217-4D72-9E42-216185CCA87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BA39A2-0FB6-463A-995D-E627458649B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AAE73E8-762A-4208-8112-C301457E7FD0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>TCNo</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Swarup3</t>
+  </si>
+  <si>
+    <t>Swarup4</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,15 +120,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F301094F-715B-4F4F-A876-93CEB5A1FD8B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,6 +518,20 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>